<commit_message>
Bump version to 1.4.6.
</commit_message>
<xml_diff>
--- a/ReserveFundBudget.xlsx
+++ b/ReserveFundBudget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>Administrative costs includes amounts to be spent on employees, insurance, utilities, repairs and maintenance, etc..</t>
+          <t xml:space="preserve">Administrative costs includes amounts to be spent on employees, insurance, utilities, repairs and maintenance, etc..</t>
         </r>
       </text>
     </comment>
@@ -50,7 +50,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>The total administrative costs includes amounts to be spent on employees, insurance, utilities, repairs and maintenance, etc..</t>
+          <t xml:space="preserve">The total administrative costs includes amounts to be spent on employees, insurance, utilities, repairs and maintenance, etc..</t>
         </r>
       </text>
     </comment>
@@ -62,7 +62,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>The repairs and maintenance costs from the administrative budget are needed to determine the minimum amount that needs to be contributed to the reserve fund.</t>
+          <t xml:space="preserve">The repairs and maintenance costs from the administrative budget are needed to determine the minimum amount that needs to be contributed to the reserve fund.</t>
         </r>
       </text>
     </comment>
@@ -74,7 +74,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>This spreadsheet assumes that inflation will be constant over the next ten years.</t>
+          <t xml:space="preserve">This spreadsheet assumes that inflation will be constant over the next ten years.</t>
         </r>
       </text>
     </comment>
@@ -85,52 +85,52 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="125">
   <si>
-    <t>ReserveFundBudget</t>
+    <t xml:space="preserve">ReserveFundBudget</t>
   </si>
   <si>
-    <t>Version: 1.4.4</t>
+    <t xml:space="preserve">Version: 1.4.6</t>
   </si>
   <si>
-    <t>This spreadsheet was created by the Trustees of the Brittany, Tokai Villas Body Corporate in</t>
+    <t xml:space="preserve">This spreadsheet was created by the Trustees of the Brittany, Tokai Villas Body Corporate in</t>
   </si>
   <si>
-    <t>consultation with Property Principals CC. It is intended to assist in drawing up a reserve fund</t>
+    <t xml:space="preserve">consultation with Property Principals CC. It is intended to assist in drawing up a reserve fund</t>
   </si>
   <si>
-    <t>budget as required by the Sectional Titles Schemes Management Regulations  and to ensure</t>
+    <t xml:space="preserve">budget as required by the Sectional Titles Schemes Management Regulations  and to ensure</t>
   </si>
   <si>
-    <t>that a Sectional Title scheme has sufficient reserves to fund its maintenance plan.</t>
+    <t xml:space="preserve">that a Sectional Title scheme has sufficient reserves to fund its maintenance plan.</t>
   </si>
   <si>
-    <t>    This program is free software: you can redistribute it and/or modify</t>
+    <t xml:space="preserve">    This program is free software: you can redistribute it and/or modify</t>
   </si>
   <si>
-    <t>    it under the terms of the GNU General Public License version 3 as published by</t>
+    <t xml:space="preserve">    it under the terms of the GNU General Public License version 3 as published by</t>
   </si>
   <si>
-    <t>    the Free Software Foundation.</t>
+    <t xml:space="preserve">    the Free Software Foundation.</t>
   </si>
   <si>
-    <t>    This program is distributed in the hope that it will be useful,</t>
+    <t xml:space="preserve">    This program is distributed in the hope that it will be useful,</t>
   </si>
   <si>
-    <t>    but WITHOUT ANY WARRANTY; without even the implied warranty of</t>
+    <t xml:space="preserve">    but WITHOUT ANY WARRANTY; without even the implied warranty of</t>
   </si>
   <si>
-    <t>    MERCHANTABILITY or FITNESS FOR A PARTICULAR PURPOSE.  See the</t>
+    <t xml:space="preserve">    MERCHANTABILITY or FITNESS FOR A PARTICULAR PURPOSE.  See the</t>
   </si>
   <si>
-    <t>    GNU General Public License for more details.</t>
+    <t xml:space="preserve">    GNU General Public License for more details.</t>
   </si>
   <si>
-    <t>    You should have received a copy of the GNU General Public License</t>
+    <t xml:space="preserve">    You should have received a copy of the GNU General Public License</t>
   </si>
   <si>
-    <t>    along with this program.  If not, see &lt;http://www.gnu.org/licenses/&gt;.</t>
+    <t xml:space="preserve">    along with this program.  If not, see &lt;http://www.gnu.org/licenses/&gt;.</t>
   </si>
   <si>
-    <t>© 2017 The Trustees of the Brittany, Tokai Villas Body Corporate</t>
+    <t xml:space="preserve">© 2017 The Trustees of the Brittany, Tokai Villas Body Corporate</t>
   </si>
   <si>
     <r>
@@ -139,7 +139,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Contact: </t>
+      <t xml:space="preserve">Contact: </t>
     </r>
     <r>
       <rPr>
@@ -148,348 +148,347 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>trustees@brittanytokaivillas.com</t>
+      <t xml:space="preserve">trustees@brittanytokaivillas.com</t>
     </r>
   </si>
   <si>
-    <t>Previous and Current Year Financials</t>
+    <t xml:space="preserve">Previous and Current Year Financials</t>
   </si>
   <si>
-    <t>This worksheet contains:</t>
+    <t xml:space="preserve">This worksheet contains:</t>
   </si>
   <si>
-    <t> - Assumptions about inflation and the interest rate applicable to the reserve fund</t>
+    <t xml:space="preserve"> - Assumptions about inflation and the interest rate applicable to the reserve fund</t>
   </si>
   <si>
-    <t> - Financial data for the previous financial year</t>
+    <t xml:space="preserve"> - Financial data for the previous financial year</t>
   </si>
   <si>
-    <t> - The total administrative budget for the current year</t>
+    <t xml:space="preserve"> - The total administrative budget for the current year</t>
   </si>
   <si>
-    <t> - The projected repairs and maintenance costs for the current year</t>
+    <t xml:space="preserve"> - The projected repairs and maintenance costs for the current year</t>
   </si>
   <si>
-    <t>In this and other worksheets, grey cells are editable and need to be populated.</t>
+    <t xml:space="preserve">In this and other worksheets, grey cells are editable and need to be populated.</t>
   </si>
   <si>
-    <t>Body Corporate Name</t>
+    <t xml:space="preserve">Body Corporate Name</t>
   </si>
   <si>
-    <t>Current Financial Year</t>
+    <t xml:space="preserve">Current Financial Year</t>
   </si>
   <si>
-    <t>Previous year administrative costs</t>
+    <t xml:space="preserve">Previous year administrative costs</t>
   </si>
   <si>
-    <t>Previous year total budget</t>
+    <t xml:space="preserve">Previous year total budget</t>
   </si>
   <si>
-    <t>Current year projected administrative costs</t>
+    <t xml:space="preserve">Current year projected administrative costs</t>
   </si>
   <si>
-    <t>Current year projected repairs and maintenance costs</t>
+    <t xml:space="preserve">Current year projected repairs and maintenance costs</t>
   </si>
   <si>
-    <t>Current year initial reserve fund amount</t>
+    <t xml:space="preserve">Current year initial reserve fund amount</t>
   </si>
   <si>
-    <t>Assumed inflation rate</t>
+    <t xml:space="preserve">Assumed inflation rate</t>
   </si>
   <si>
-    <t>Bank deposit interest rate</t>
+    <t xml:space="preserve">Bank deposit interest rate</t>
   </si>
   <si>
-    <t>Ten Year Plan</t>
+    <t xml:space="preserve">Ten Year Plan</t>
   </si>
   <si>
-    <t>This spreadsheet contains items that need to be budgeted for over the next 10 years.</t>
+    <t xml:space="preserve">This spreadsheet contains items that need to be budgeted for over the next 10 years.</t>
   </si>
   <si>
-    <t>Budgeted items would include:</t>
+    <t xml:space="preserve">Budgeted items would include:</t>
   </si>
   <si>
-    <t> - Repainting  </t>
+    <t xml:space="preserve"> - Repainting  </t>
   </si>
   <si>
-    <t> - Security enhancements</t>
+    <t xml:space="preserve"> - Security enhancements</t>
   </si>
   <si>
-    <t> - Wall and fence repairs and replacement</t>
+    <t xml:space="preserve"> - Wall and fence repairs and replacement</t>
   </si>
   <si>
-    <t> - Gutter and drainpipe repairs and replacement</t>
+    <t xml:space="preserve"> - Gutter and drainpipe repairs and replacement</t>
   </si>
   <si>
-    <t>It is possible to specify a range of years over which maintenance work must be done.</t>
+    <t xml:space="preserve">It is possible to specify a range of years over which maintenance work must be done.</t>
   </si>
   <si>
-    <t>For example, it might be that gutters will be replaced over two years. It is also possible to</t>
+    <t xml:space="preserve">For example, it might be that gutters will be replaced over two years. It is also possible to</t>
   </si>
   <si>
-    <t>specify that some maintenance work must be done every N years; e.g. that woodwork</t>
+    <t xml:space="preserve">specify that some maintenance work must be done every N years; e.g. that woodwork</t>
   </si>
   <si>
-    <t>repainting happens every 4 years.</t>
+    <t xml:space="preserve">repainting happens every 4 years.</t>
   </si>
   <si>
-    <t>Item</t>
+    <t xml:space="preserve">Item</t>
   </si>
   <si>
-    <t>Start Year</t>
+    <t xml:space="preserve">Start Year</t>
   </si>
   <si>
-    <t>End Year</t>
+    <t xml:space="preserve">End Year</t>
   </si>
   <si>
-    <t>Step (years)</t>
+    <t xml:space="preserve">Step (years)</t>
   </si>
   <si>
-    <t>Annual amount (real)</t>
+    <t xml:space="preserve">Annual amount (real)</t>
   </si>
   <si>
-    <t>Wiring, lighting &amp; electrical</t>
+    <t xml:space="preserve">Wiring, lighting &amp; electrical</t>
   </si>
   <si>
-    <t>Plumbing, drainage &amp; storm-water system</t>
+    <t xml:space="preserve">Plumbing, drainage &amp; storm-water system</t>
   </si>
   <si>
-    <t>Painting &amp; waterproofing</t>
+    <t xml:space="preserve">Painting &amp; waterproofing</t>
   </si>
   <si>
-    <t>Security</t>
+    <t xml:space="preserve">Security</t>
   </si>
   <si>
-    <t>Recreational facilities</t>
+    <t xml:space="preserve">Recreational facilities</t>
   </si>
   <si>
-    <t>Communication systems</t>
+    <t xml:space="preserve">Communication systems</t>
   </si>
   <si>
-    <t>Parking, roadways &amp; paving</t>
+    <t xml:space="preserve">Parking, roadways &amp; paving</t>
   </si>
   <si>
-    <t>Roofing</t>
+    <t xml:space="preserve">Roofing</t>
   </si>
   <si>
-    <t>Lifts</t>
+    <t xml:space="preserve">Lifts</t>
   </si>
   <si>
-    <t>Carpeting &amp; Furnishings</t>
+    <t xml:space="preserve">Carpeting &amp; Furnishings</t>
   </si>
   <si>
-    <t>Heating &amp; cooling facilities</t>
+    <t xml:space="preserve">Heating &amp; cooling facilities</t>
   </si>
   <si>
-    <t>Other</t>
+    <t xml:space="preserve">Other</t>
   </si>
   <si>
-    <t>Naive Current Financial Year Planner</t>
+    <t xml:space="preserve">Naive Current Financial Year Planner</t>
   </si>
   <si>
-    <t>This worksheet generates a naive recommendation for the budget</t>
+    <t xml:space="preserve">This worksheet generates a naive recommendation for the budget</t>
   </si>
   <si>
-    <t>change for the current financial year over the previous year.</t>
+    <t xml:space="preserve">change for the current financial year over the previous year.</t>
   </si>
   <si>
-    <t>The recommendation is based on a formula in Section 22 of the</t>
+    <t xml:space="preserve">The recommendation is based on a formula in Section 22 of the</t>
   </si>
   <si>
-    <t>Management Rules of the STSMA Regulations. The recommendation</t>
+    <t xml:space="preserve">Management Rules of the STSMA Regulations. The recommendation</t>
   </si>
   <si>
-    <t>is aggressive since it gets a BC into compliance in one year meaning</t>
+    <t xml:space="preserve">is aggressive since it gets a BC into compliance in one year meaning</t>
   </si>
   <si>
-    <t>that levies may need to be reduced in real terms in subsequent</t>
+    <t xml:space="preserve">that levies may need to be reduced in real terms in subsequent</t>
   </si>
   <si>
-    <t>years.</t>
+    <t xml:space="preserve">years.</t>
   </si>
   <si>
-    <t>Actual initial reserve fund amount</t>
+    <t xml:space="preserve">Actual initial reserve fund amount</t>
   </si>
   <si>
-    <t>Recommended initial reserve fund amount</t>
+    <t xml:space="preserve">Recommended initial reserve fund amount</t>
   </si>
   <si>
-    <t>Difference between actual and recommended</t>
+    <t xml:space="preserve">Difference between actual and recommended</t>
   </si>
   <si>
-    <t>Recommended reserve fund contribution</t>
+    <t xml:space="preserve">Recommended reserve fund contribution</t>
   </si>
   <si>
-    <t>Recommended real budget change</t>
+    <t xml:space="preserve">Recommended real budget change</t>
   </si>
   <si>
-    <t>Recommended nominal budget change</t>
+    <t xml:space="preserve">Recommended nominal budget change</t>
   </si>
   <si>
-    <t>Recommended final reserve fund amount</t>
+    <t xml:space="preserve">Recommended final reserve fund amount</t>
   </si>
   <si>
-    <t>Ideal res.</t>
+    <t xml:space="preserve">Ideal res.</t>
   </si>
   <si>
-    <t>Sum ideal</t>
+    <t xml:space="preserve">Sum ideal</t>
   </si>
   <si>
-    <t>actual/ideal</t>
+    <t xml:space="preserve">actual/ideal</t>
   </si>
   <si>
-    <t>Res. Con.</t>
+    <t xml:space="preserve">Res. Con.</t>
   </si>
   <si>
-    <t>Total res. c.</t>
+    <t xml:space="preserve">Total res. c.</t>
   </si>
   <si>
-    <t>Planning and Projections</t>
+    <t xml:space="preserve">Planning and Projections</t>
   </si>
   <si>
-    <t>This worksheet is used to determine what year on year increases</t>
+    <t xml:space="preserve">This worksheet is used to determine what year on year increases</t>
   </si>
   <si>
-    <t>should be considered over the next ten years. The changes are</t>
+    <t xml:space="preserve">should be considered over the next ten years. The changes are</t>
   </si>
   <si>
-    <t>expressed in real terms, i.e. constant currency ignoring inflation.</t>
+    <t xml:space="preserve">expressed in real terms, i.e. constant currency ignoring inflation.</t>
   </si>
   <si>
-    <t>If the annual changes are close to zero, a Sectional Title scheme</t>
+    <t xml:space="preserve">If the annual changes are close to zero, a Sectional Title scheme</t>
   </si>
   <si>
-    <t>would be appear to be in sound financial health and residents</t>
+    <t xml:space="preserve">would be appear to be in sound financial health and residents</t>
   </si>
   <si>
-    <t>should not be unpleasantly surprised by large levy fluctuations.</t>
+    <t xml:space="preserve">should not be unpleasantly surprised by large levy fluctuations.</t>
   </si>
   <si>
-    <t>If either of the “Reserve fund budget OK?” or “Final reserve OK?”</t>
+    <t xml:space="preserve">If either of the “Reserve fund budget OK?” or “Final reserve OK?”</t>
   </si>
   <si>
-    <t>entries shows “NOT OK”, it should be taken as a warning that</t>
+    <t xml:space="preserve">entries shows “NOT OK”, it should be taken as a warning that</t>
   </si>
   <si>
-    <t>the financial planning may be inadequate for the long-term</t>
+    <t xml:space="preserve">the financial planning may be inadequate for the long-term</t>
   </si>
   <si>
-    <t>maintenance of a scheme.</t>
+    <t xml:space="preserve">maintenance of a scheme.</t>
   </si>
   <si>
-    <t>Year</t>
+    <t xml:space="preserve">Year</t>
   </si>
   <si>
-    <t>Proposed budget change real (%)</t>
+    <t xml:space="preserve">Proposed budget change real (%)</t>
   </si>
   <si>
-    <t>Proposed budget change nominal (%)</t>
+    <t xml:space="preserve">Proposed budget change nominal (%)</t>
   </si>
   <si>
-    <t>Initial reserve (nominal)</t>
+    <t xml:space="preserve">Initial reserve (nominal)</t>
   </si>
   <si>
-    <t>Administrative budget (nominal)</t>
+    <t xml:space="preserve">Administrative budget (nominal)</t>
   </si>
   <si>
-    <t>Repairs &amp; Maintenance (nominal)</t>
+    <t xml:space="preserve">Repairs &amp; Maintenance (nominal)</t>
   </si>
   <si>
-    <t>Total budget (nominal)</t>
+    <t xml:space="preserve">Total budget (nominal)</t>
   </si>
   <si>
-    <t>Reserve fund budget (nominal)</t>
+    <t xml:space="preserve">Reserve fund budget (nominal)</t>
   </si>
   <si>
-    <t>Additional months of fund contributions needed for current year</t>
+    <t xml:space="preserve">Additional months of fund contributions needed for current year</t>
   </si>
   <si>
-    <t>Reserve fund budget OK?</t>
+    <t xml:space="preserve">Reserve fund budget OK?</t>
   </si>
   <si>
-    <t>Reserve fund spending (nominal)</t>
+    <t xml:space="preserve">Reserve fund spending (nominal)</t>
   </si>
   <si>
-    <t>Final reserve (nominal)</t>
+    <t xml:space="preserve">Final reserve (nominal)</t>
   </si>
   <si>
-    <t>Final reserve (months)</t>
+    <t xml:space="preserve">Final reserve (months)</t>
   </si>
   <si>
-    <t>Final reserve OK?</t>
+    <t xml:space="preserve">Final reserve OK?</t>
   </si>
   <si>
-    <t>Budget Summary</t>
+    <t xml:space="preserve">Budget Summary</t>
   </si>
   <si>
-    <t>This worksheet summarizes the changes in the budget and</t>
+    <t xml:space="preserve">This worksheet summarizes the changes in the budget and</t>
   </si>
   <si>
-    <t>reserves for the current year over the previous financial</t>
+    <t xml:space="preserve">reserves for the current year over the previous financial</t>
   </si>
   <si>
-    <t>year.</t>
+    <t xml:space="preserve">year.</t>
   </si>
   <si>
-    <t>Administrative budget</t>
+    <t xml:space="preserve">Administrative budget</t>
   </si>
   <si>
-    <t>Reserve fund budget</t>
+    <t xml:space="preserve">Reserve fund budget</t>
   </si>
   <si>
-    <t>Total budget</t>
+    <t xml:space="preserve">Total budget</t>
   </si>
   <si>
-    <t>Reserve fund budget / Total budget</t>
+    <t xml:space="preserve">Reserve fund budget / Total budget</t>
   </si>
   <si>
-    <t>Previous year's total budget</t>
+    <t xml:space="preserve">Previous year's total budget</t>
   </si>
   <si>
-    <t>Total budget change from previous year (%)</t>
+    <t xml:space="preserve">Total budget change from previous year (%)</t>
   </si>
   <si>
-    <t>Reserve Fund Summary</t>
+    <t xml:space="preserve">Reserve Fund Summary</t>
   </si>
   <si>
-    <t>Initial reserves</t>
+    <t xml:space="preserve">Initial reserves</t>
   </si>
   <si>
-    <t>Recommended initial reserves</t>
+    <t xml:space="preserve">Recommended initial reserves</t>
   </si>
   <si>
-    <t>Actual versus recommended difference</t>
+    <t xml:space="preserve">Actual versus recommended difference</t>
   </si>
   <si>
-    <t>Actual versus recommended difference (%)</t>
+    <t xml:space="preserve">Actual versus recommended difference (%)</t>
   </si>
   <si>
-    <t>Projected final reserves at year end</t>
+    <t xml:space="preserve">Projected final reserves at year end</t>
   </si>
   <si>
-    <t>Recommended final reserves</t>
+    <t xml:space="preserve">Recommended final reserves</t>
   </si>
   <si>
-    <t>Percentage change in reserves</t>
+    <t xml:space="preserve">Percentage change in reserves</t>
   </si>
   <si>
-    <t>Reserves in months</t>
+    <t xml:space="preserve">Reserves in months</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  <numFmts count="8">
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$R-1C09]\ #,##0;[RED][$R-1C09]\-#,##0"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="[$R-1C09]\ #,##0;[RED][$R-1C09]\-#,##0;&quot;&quot;"/>
     <numFmt numFmtId="168" formatCode="0.0%;[RED]\-0.0%"/>
-    <numFmt numFmtId="169" formatCode="[$R-1C09]\ #,##0;[$R-1C09]\-#,##0"/>
-    <numFmt numFmtId="170" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="0.0;[RED]\-0.0"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0;[RED]\-0.0"/>
+    <numFmt numFmtId="171" formatCode="0.0%"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -557,13 +556,13 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -622,7 +621,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -735,19 +734,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -771,19 +762,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -799,15 +790,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1022,7 +1017,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1195,7 +1190,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -4814,7 +4809,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -4830,7 +4825,7 @@
   <dimension ref="A1:AY94"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4976,20 +4971,20 @@
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
-      <c r="E15" s="28" t="e">
+      <c r="E15" s="26" t="e">
         <f aca="false">AY22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="29"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="28"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="25" t="s">
         <v>73</v>
       </c>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
-      <c r="E16" s="30" t="e">
+      <c r="E16" s="29" t="e">
         <f aca="false">E17-'Current Financials'!B18</f>
         <v>#DIV/0!</v>
       </c>
@@ -5001,7 +4996,7 @@
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="31" t="e">
+      <c r="E17" s="27" t="e">
         <f aca="false">('Current Financials'!$B$15+$E$15)/'Current Financials'!$B$14-1</f>
         <v>#DIV/0!</v>
       </c>
@@ -17470,7 +17465,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -17573,7 +17568,7 @@
       <c r="B14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="30" t="s">
         <v>92</v>
       </c>
       <c r="B15" s="18" t="n">
@@ -17618,37 +17613,37 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" s="34" t="n">
+      <c r="B16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17656,43 +17651,43 @@
       <c r="A17" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="35" t="n">
+      <c r="B17" s="33" t="n">
         <f aca="false">B16+'Current Financials'!$B$18</f>
         <v>0</v>
       </c>
-      <c r="C17" s="35" t="n">
+      <c r="C17" s="33" t="n">
         <f aca="false">C16+'Current Financials'!$B$18</f>
         <v>0</v>
       </c>
-      <c r="D17" s="35" t="n">
+      <c r="D17" s="33" t="n">
         <f aca="false">D16+'Current Financials'!$B$18</f>
         <v>0</v>
       </c>
-      <c r="E17" s="35" t="n">
+      <c r="E17" s="33" t="n">
         <f aca="false">E16+'Current Financials'!$B$18</f>
         <v>0</v>
       </c>
-      <c r="F17" s="35" t="n">
+      <c r="F17" s="33" t="n">
         <f aca="false">F16+'Current Financials'!$B$18</f>
         <v>0</v>
       </c>
-      <c r="G17" s="35" t="n">
+      <c r="G17" s="33" t="n">
         <f aca="false">G16+'Current Financials'!$B$18</f>
         <v>0</v>
       </c>
-      <c r="H17" s="35" t="n">
+      <c r="H17" s="33" t="n">
         <f aca="false">H16+'Current Financials'!$B$18</f>
         <v>0</v>
       </c>
-      <c r="I17" s="35" t="n">
+      <c r="I17" s="33" t="n">
         <f aca="false">I16+'Current Financials'!$B$18</f>
         <v>0</v>
       </c>
-      <c r="J17" s="35" t="n">
+      <c r="J17" s="33" t="n">
         <f aca="false">J16+'Current Financials'!$B$18</f>
         <v>0</v>
       </c>
-      <c r="K17" s="35" t="n">
+      <c r="K17" s="33" t="n">
         <f aca="false">K16+'Current Financials'!$B$18</f>
         <v>0</v>
       </c>
@@ -17836,43 +17831,43 @@
       <c r="A21" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="36" t="n">
+      <c r="B21" s="34" t="n">
         <f aca="false">'Current Financials'!B14*(1+B17)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="36" t="n">
+      <c r="C21" s="34" t="n">
         <f aca="false">B21*(1+C17)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="36" t="n">
+      <c r="D21" s="34" t="n">
         <f aca="false">C21*(1+D17)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="36" t="n">
+      <c r="E21" s="34" t="n">
         <f aca="false">D21*(1+E17)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="36" t="n">
+      <c r="F21" s="34" t="n">
         <f aca="false">E21*(1+F17)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="36" t="n">
+      <c r="G21" s="34" t="n">
         <f aca="false">F21*(1+G17)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="36" t="n">
+      <c r="H21" s="34" t="n">
         <f aca="false">G21*(1+H17)</f>
         <v>0</v>
       </c>
-      <c r="I21" s="36" t="n">
+      <c r="I21" s="34" t="n">
         <f aca="false">H21*(1+I17)</f>
         <v>0</v>
       </c>
-      <c r="J21" s="36" t="n">
+      <c r="J21" s="34" t="n">
         <f aca="false">I21*(1+J17)</f>
         <v>0</v>
       </c>
-      <c r="K21" s="36" t="n">
+      <c r="K21" s="34" t="n">
         <f aca="false">J21*(1+K17)</f>
         <v>0</v>
       </c>
@@ -17926,43 +17921,43 @@
       <c r="A23" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="37" t="n">
+      <c r="B23" s="35" t="n">
         <f aca="false">IF(B18&gt;=B25,0,(B25-B18)/(B22/12))</f>
         <v>0</v>
       </c>
-      <c r="C23" s="37" t="n">
+      <c r="C23" s="35" t="n">
         <f aca="false">IF(C18&gt;=C25,0,(C25-C18)/(C22/12))</f>
         <v>0</v>
       </c>
-      <c r="D23" s="37" t="n">
+      <c r="D23" s="35" t="n">
         <f aca="false">IF(D18&gt;=D25,0,(D25-D18)/(D22/12))</f>
         <v>0</v>
       </c>
-      <c r="E23" s="37" t="n">
+      <c r="E23" s="35" t="n">
         <f aca="false">IF(E18&gt;=E25,0,(E25-E18)/(E22/12))</f>
         <v>0</v>
       </c>
-      <c r="F23" s="37" t="n">
+      <c r="F23" s="35" t="n">
         <f aca="false">IF(F18&gt;=F25,0,(F25-F18)/(F22/12))</f>
         <v>0</v>
       </c>
-      <c r="G23" s="37" t="n">
+      <c r="G23" s="35" t="n">
         <f aca="false">IF(G18&gt;=G25,0,(G25-G18)/(G22/12))</f>
         <v>0</v>
       </c>
-      <c r="H23" s="37" t="n">
+      <c r="H23" s="35" t="n">
         <f aca="false">IF(H18&gt;=H25,0,(H25-H18)/(H22/12))</f>
         <v>0</v>
       </c>
-      <c r="I23" s="37" t="n">
+      <c r="I23" s="35" t="n">
         <f aca="false">IF(I18&gt;=I25,0,(I25-I18)/(I22/12))</f>
         <v>0</v>
       </c>
-      <c r="J23" s="37" t="n">
+      <c r="J23" s="35" t="n">
         <f aca="false">IF(J18&gt;=J25,0,(J25-J18)/(J22/12))</f>
         <v>0</v>
       </c>
-      <c r="K23" s="37" t="n">
+      <c r="K23" s="35" t="n">
         <f aca="false">IF(K18&gt;=K25,0,(K25-K18)/(K22/12))</f>
         <v>0</v>
       </c>
@@ -17971,43 +17966,43 @@
       <c r="A24" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="38" t="str">
+      <c r="B24" s="36" t="str">
         <f aca="false">IF(B18&gt;='Current Financials'!$B$13,"",IF(B18&gt;='Current Financials'!$B$13/4,IF(B22&gt;=B20, "", "NOT OK1"), IF(B22&gt;=0.15*B19, "", "NOT OK2")))</f>
         <v/>
       </c>
-      <c r="C24" s="38" t="str">
+      <c r="C24" s="36" t="str">
         <f aca="false">IF(C18&gt;=B19,"",IF(C18&gt;=B19/4,IF(C22&gt;=C20, "", "NOT OK1"), IF(C22&gt;=0.15*C19, "", "NOT OK2")))</f>
         <v/>
       </c>
-      <c r="D24" s="38" t="str">
+      <c r="D24" s="36" t="str">
         <f aca="false">IF(D18&gt;=C19,"",IF(D18&gt;=C19/4,IF(D22&gt;=D20, "", "NOT OK1"), IF(D22&gt;=0.15*D19, "", "NOT OK2")))</f>
         <v/>
       </c>
-      <c r="E24" s="38" t="str">
+      <c r="E24" s="36" t="str">
         <f aca="false">IF(E18&gt;=D19,"",IF(E18&gt;=D19/4,IF(E22&gt;=E20, "", "NOT OK1"), IF(E22&gt;=0.15*E19, "", "NOT OK2")))</f>
         <v/>
       </c>
-      <c r="F24" s="38" t="str">
+      <c r="F24" s="36" t="str">
         <f aca="false">IF(F18&gt;=E19,"",IF(F18&gt;=E19/4,IF(F22&gt;=F20, "", "NOT OK1"), IF(F22&gt;=0.15*F19, "", "NOT OK2")))</f>
         <v/>
       </c>
-      <c r="G24" s="38" t="str">
+      <c r="G24" s="36" t="str">
         <f aca="false">IF(G18&gt;=F19,"",IF(G18&gt;=F19/4,IF(G22&gt;=G20, "", "NOT OK1"), IF(G22&gt;=0.15*G19, "", "NOT OK2")))</f>
         <v/>
       </c>
-      <c r="H24" s="38" t="str">
+      <c r="H24" s="36" t="str">
         <f aca="false">IF(H18&gt;=G19,"",IF(H18&gt;=G19/4,IF(H22&gt;=H20, "", "NOT OK1"), IF(H22&gt;=0.15*H19, "", "NOT OK2")))</f>
         <v/>
       </c>
-      <c r="I24" s="38" t="str">
+      <c r="I24" s="36" t="str">
         <f aca="false">IF(I18&gt;=H19,"",IF(I18&gt;=H19/4,IF(I22&gt;=I20, "", "NOT OK1"), IF(I22&gt;=0.15*I19, "", "NOT OK2")))</f>
         <v/>
       </c>
-      <c r="J24" s="38" t="str">
+      <c r="J24" s="36" t="str">
         <f aca="false">IF(J18&gt;=I19,"",IF(J18&gt;=I19/4,IF(J22&gt;=J20, "", "NOT OK1"), IF(J22&gt;=0.15*J19, "", "NOT OK2")))</f>
         <v/>
       </c>
-      <c r="K24" s="38" t="str">
+      <c r="K24" s="36" t="str">
         <f aca="false">IF(K18&gt;=J19,"",IF(K18&gt;=J19/4,IF(K22&gt;=K20, "", "NOT OK1"), IF(K22&gt;=0.15*K19, "", "NOT OK2")))</f>
         <v/>
       </c>
@@ -18061,43 +18056,43 @@
       <c r="A26" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="36" t="n">
+      <c r="B26" s="34" t="n">
         <f aca="false">B18+B22-B25+(2*B18+B22-B25)/2*'Current Financials'!$B$19</f>
         <v>0</v>
       </c>
-      <c r="C26" s="36" t="n">
+      <c r="C26" s="34" t="n">
         <f aca="false">C18+C22-C25+(2*C18+C22-C25)/2*'Current Financials'!$B$19</f>
         <v>0</v>
       </c>
-      <c r="D26" s="36" t="n">
+      <c r="D26" s="34" t="n">
         <f aca="false">D18+D22-D25+(2*D18+D22-D25)/2*'Current Financials'!$B$19</f>
         <v>0</v>
       </c>
-      <c r="E26" s="36" t="n">
+      <c r="E26" s="34" t="n">
         <f aca="false">E18+E22-E25+(2*E18+E22-E25)/2*'Current Financials'!$B$19</f>
         <v>0</v>
       </c>
-      <c r="F26" s="36" t="n">
+      <c r="F26" s="34" t="n">
         <f aca="false">F18+F22-F25+(2*F18+F22-F25)/2*'Current Financials'!$B$19</f>
         <v>0</v>
       </c>
-      <c r="G26" s="36" t="n">
+      <c r="G26" s="34" t="n">
         <f aca="false">G18+G22-G25+(2*G18+G22-G25)/2*'Current Financials'!$B$19</f>
         <v>0</v>
       </c>
-      <c r="H26" s="36" t="n">
+      <c r="H26" s="34" t="n">
         <f aca="false">H18+H22-H25+(2*H18+H22-H25)/2*'Current Financials'!$B$19</f>
         <v>0</v>
       </c>
-      <c r="I26" s="36" t="n">
+      <c r="I26" s="34" t="n">
         <f aca="false">I18+I22-I25+(2*I18+I22-I25)/2*'Current Financials'!$B$19</f>
         <v>0</v>
       </c>
-      <c r="J26" s="36" t="n">
+      <c r="J26" s="34" t="n">
         <f aca="false">J18+J22-J25+(2*J18+J22-J25)/2*'Current Financials'!$B$19</f>
         <v>0</v>
       </c>
-      <c r="K26" s="36" t="n">
+      <c r="K26" s="34" t="n">
         <f aca="false">K18+K22-K25+(2*K18+K22-K25)/2*'Current Financials'!$B$19</f>
         <v>0</v>
       </c>
@@ -18106,43 +18101,43 @@
       <c r="A27" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="39" t="e">
+      <c r="B27" s="37" t="e">
         <f aca="false">B26/B19*12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C27" s="39" t="e">
+      <c r="C27" s="37" t="e">
         <f aca="false">C26/C19*12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D27" s="39" t="e">
+      <c r="D27" s="37" t="e">
         <f aca="false">D26/D19*12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E27" s="39" t="e">
+      <c r="E27" s="37" t="e">
         <f aca="false">E26/E19*12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F27" s="39" t="e">
+      <c r="F27" s="37" t="e">
         <f aca="false">F26/F19*12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G27" s="39" t="e">
+      <c r="G27" s="37" t="e">
         <f aca="false">G26/G19*12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H27" s="39" t="e">
+      <c r="H27" s="37" t="e">
         <f aca="false">H26/H19*12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I27" s="39" t="e">
+      <c r="I27" s="37" t="e">
         <f aca="false">I26/I19*12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J27" s="39" t="e">
+      <c r="J27" s="37" t="e">
         <f aca="false">J26/J19*12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K27" s="39" t="e">
+      <c r="K27" s="37" t="e">
         <f aca="false">K26/K19*12</f>
         <v>#DIV/0!</v>
       </c>
@@ -18151,43 +18146,43 @@
       <c r="A28" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="38" t="str">
+      <c r="B28" s="36" t="str">
         <f aca="false">IF(B26&lt;0, "NOT OK!", IF(B26&gt;=B19/4,"","Low"))</f>
         <v/>
       </c>
-      <c r="C28" s="38" t="str">
+      <c r="C28" s="36" t="str">
         <f aca="false">IF(C26&lt;0, "NOT OK!", IF(C26&gt;=C19/4,"","Low"))</f>
         <v/>
       </c>
-      <c r="D28" s="38" t="str">
+      <c r="D28" s="36" t="str">
         <f aca="false">IF(D26&lt;0, "NOT OK!", IF(D26&gt;=D19/4,"","Low"))</f>
         <v/>
       </c>
-      <c r="E28" s="38" t="str">
+      <c r="E28" s="36" t="str">
         <f aca="false">IF(E26&lt;0, "NOT OK!", IF(E26&gt;=E19/4,"","Low"))</f>
         <v/>
       </c>
-      <c r="F28" s="38" t="str">
+      <c r="F28" s="36" t="str">
         <f aca="false">IF(F26&lt;0, "NOT OK!", IF(F26&gt;=F19/4,"","Low"))</f>
         <v/>
       </c>
-      <c r="G28" s="38" t="str">
+      <c r="G28" s="36" t="str">
         <f aca="false">IF(G26&lt;0, "NOT OK!", IF(G26&gt;=G19/4,"","Low"))</f>
         <v/>
       </c>
-      <c r="H28" s="38" t="str">
+      <c r="H28" s="36" t="str">
         <f aca="false">IF(H26&lt;0, "NOT OK!", IF(H26&gt;=H19/4,"","Low"))</f>
         <v/>
       </c>
-      <c r="I28" s="38" t="str">
+      <c r="I28" s="36" t="str">
         <f aca="false">IF(I26&lt;0, "NOT OK!", IF(I26&gt;=I19/4,"","Low"))</f>
         <v/>
       </c>
-      <c r="J28" s="38" t="str">
+      <c r="J28" s="36" t="str">
         <f aca="false">IF(J26&lt;0, "NOT OK!", IF(J26&gt;=J19/4,"","Low"))</f>
         <v/>
       </c>
-      <c r="K28" s="38" t="str">
+      <c r="K28" s="36" t="str">
         <f aca="false">IF(K26&lt;0, "NOT OK!", IF(K26&gt;=K19/4,"","Low"))</f>
         <v/>
       </c>
@@ -18201,7 +18196,7 @@
   <sheetProtection sheet="true" objects="true" scenarios="true" selectLockedCells="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -18264,52 +18259,52 @@
       <c r="B7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="41"/>
+      <c r="B8" s="39"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="43" t="n">
+      <c r="B9" s="41" t="n">
         <f aca="false">'Current Financials'!B15</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="43" t="n">
+      <c r="B10" s="41" t="n">
         <f aca="false">'Planning and Projections'!B22</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="43" t="n">
+      <c r="B11" s="41" t="n">
         <f aca="false">'Planning and Projections'!B21</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="44" t="e">
+      <c r="B12" s="42" t="e">
         <f aca="false">B10/B11</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="43" t="n">
+      <c r="B13" s="41" t="n">
         <f aca="false">'Current Financials'!B14</f>
         <v>0</v>
       </c>
@@ -18318,20 +18313,20 @@
       <c r="A14" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B14" s="31" t="e">
+      <c r="B14" s="43" t="e">
         <f aca="false">B11/'Current Financials'!B14-1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="25"/>
-      <c r="B15" s="31"/>
+      <c r="B15" s="43"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="31"/>
+      <c r="B16" s="43"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="25" t="s">
@@ -18426,7 +18421,7 @@
       <c r="A28" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="46" t="e">
+      <c r="B28" s="45" t="e">
         <f aca="false">'Planning and Projections'!B27</f>
         <v>#DIV/0!</v>
       </c>
@@ -18442,7 +18437,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>